<commit_message>
implemented JS progress bar, closes #37 also fixed some bugs in check_button
</commit_message>
<xml_diff>
--- a/documentation/Example files/email.xlsx
+++ b/documentation/Example files/email.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>typ</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>YOUR EMAIL BRO</t>
+  </si>
+  <si>
+    <t>invite_me</t>
+  </si>
+  <si>
+    <t>You may invite me.</t>
+  </si>
+  <si>
+    <t>check_button</t>
   </si>
 </sst>
 </file>
@@ -485,7 +494,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -575,6 +584,17 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:18">

</xml_diff>